<commit_message>
Added more details to GVED
</commit_message>
<xml_diff>
--- a/Data/table_feature.xlsx
+++ b/Data/table_feature.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12380" yWindow="2040" windowWidth="22420" windowHeight="14640" xr2:uid="{A271DACC-8F26-6843-85C1-F616E817FD05}"/>
+    <workbookView xWindow="2340" yWindow="460" windowWidth="22420" windowHeight="14640" xr2:uid="{A271DACC-8F26-6843-85C1-F616E817FD05}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="34">
   <si>
     <t>Pattern</t>
   </si>
@@ -111,14 +112,46 @@
   </si>
   <si>
     <t>intSmall2-1-2</t>
+  </si>
+  <si>
+    <t>Feature</t>
+  </si>
+  <si>
+    <t>Index</t>
+  </si>
+  <si>
+    <t>Counted in Code1</t>
+  </si>
+  <si>
+    <t>Counted in Code2</t>
+  </si>
+  <si>
+    <t>To be continued…</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -134,7 +167,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -142,16 +175,82 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -468,165 +567,334 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{821EAE7F-DFDB-B949-94E7-74C0B7BC3FEA}">
-  <dimension ref="B5:M9"/>
+  <dimension ref="B5:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="2" max="2" width="12.33203125" customWidth="1"/>
     <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="16.1640625" customWidth="1"/>
+    <col min="5" max="5" width="15.5" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2" t="s">
+      <c r="C5" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="B7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="B8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="4"/>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-    </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B14" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C14" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D14" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I14">
+        <v>7</v>
+      </c>
+      <c r="J14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="B15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" s="5"/>
+    </row>
+    <row r="16" spans="2:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="B16" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="5"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B17" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G17" s="4"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B20" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B21" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="4">
+        <v>1</v>
+      </c>
+      <c r="D21" s="4">
+        <v>1</v>
+      </c>
+      <c r="E21" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B22" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="4">
+        <v>2</v>
+      </c>
+      <c r="D22" s="4">
+        <v>1</v>
+      </c>
+      <c r="E22" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B23" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F6" t="s">
+      <c r="C23" s="4">
+        <v>3</v>
+      </c>
+      <c r="D23" s="4">
+        <v>1</v>
+      </c>
+      <c r="E23" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B24" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G6" t="s">
+      <c r="C24" s="4">
+        <v>4</v>
+      </c>
+      <c r="D24" s="4">
+        <v>1</v>
+      </c>
+      <c r="E24" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B25" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H6" t="s">
-        <v>2</v>
-      </c>
-      <c r="I6" t="s">
-        <v>3</v>
-      </c>
-      <c r="J6" t="s">
-        <v>4</v>
-      </c>
-      <c r="K6" t="s">
+      <c r="C25" s="4">
+        <v>5</v>
+      </c>
+      <c r="D25" s="4">
+        <v>1</v>
+      </c>
+      <c r="E25" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B26" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="L6" t="s">
+      <c r="C26" s="4">
         <v>6</v>
       </c>
-      <c r="M6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="2:13" ht="32" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
+      <c r="D26" s="4">
+        <v>0</v>
+      </c>
+      <c r="E26" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="B27" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" s="4">
         <v>7</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D27" s="4">
+        <v>1</v>
+      </c>
+      <c r="E27" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B28" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" s="4">
         <v>8</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" t="s">
-        <v>7</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="M7" s="1"/>
-    </row>
-    <row r="8" spans="2:13" ht="48" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J8" s="1"/>
-    </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H9" t="s">
-        <v>16</v>
-      </c>
-      <c r="I9" t="s">
-        <v>17</v>
-      </c>
-      <c r="J9" t="s">
-        <v>18</v>
-      </c>
-      <c r="K9" t="s">
-        <v>26</v>
-      </c>
-      <c r="L9" t="s">
-        <v>27</v>
-      </c>
+      <c r="D28" s="4">
+        <v>0</v>
+      </c>
+      <c r="E28" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B29" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="C5:G5"/>
-    <mergeCell ref="H5:L5"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="B29:E29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>